<commit_message>
Added STL's and Additional Parts
Added STL's and Additional Images
</commit_message>
<xml_diff>
--- a/BOM/ES25 BOM.xlsx
+++ b/BOM/ES25 BOM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Documents\04 - Github\Eustathios Spider V2.5_1\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Documents\04 - Github\Eustathios-Spider-V2.5\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{C231A055-2E8D-4691-A9C5-7A7A0C5DAD30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{86DCCD27-8181-45E5-82CF-C09A532D38B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -91,12 +91,6 @@
     <t>SFJ10-435</t>
   </si>
   <si>
-    <t>Z_Axis_Shaft_Mount_A</t>
-  </si>
-  <si>
-    <t>Z_Axis_Shaft_Mount_B</t>
-  </si>
-  <si>
     <t>M5 Nylock Nut</t>
   </si>
   <si>
@@ -181,9 +175,6 @@
     <t>Bondtech_BMG</t>
   </si>
   <si>
-    <t>X(NEW) Endstop Mount</t>
-  </si>
-  <si>
     <t>Micro Switch Button</t>
   </si>
   <si>
@@ -202,12 +193,6 @@
     <t>TMC2209</t>
   </si>
   <si>
-    <t>Outlet_Switch_Mount</t>
-  </si>
-  <si>
-    <t>Z(NEW) Endstop Mount</t>
-  </si>
-  <si>
     <t>4mm x 16mm SST BSC</t>
   </si>
   <si>
@@ -586,9 +571,6 @@
     <t>IEC 10A 250V Fused Receptical with Switch</t>
   </si>
   <si>
-    <t>Bearing_Holder with Pass Through</t>
-  </si>
-  <si>
     <t>3D Printed 6900-2RS Bearing Holder</t>
   </si>
   <si>
@@ -686,9 +668,6 @@
   </si>
   <si>
     <t>https://www.aliexpress.com/item/32811240720.html?spm=2114.12010610.8148356.3.510d6ff09MSsfJ</t>
-  </si>
-  <si>
-    <t>XY_External_Motor_Mount</t>
   </si>
   <si>
     <t>3D printed X / Y Motor Mount</t>
@@ -960,108 +939,6 @@
         <family val="2"/>
       </rPr>
       <t>V3</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">SKR_1.3 / 1.4 Controller </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>Mount</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>XY_Side_Carriage_Za</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>ne_V2.5_Rev2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>XY_Side_Carriage_Zan</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>e_V2.5_Rev2 (Mirrored)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Y (New) Endstop </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="SWGDT"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>Mount</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Z_Axis_Bed_Support </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="SWGDT"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>V2.5</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Z_Integrated_Leadsc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>rew_Motor_Mount</t>
     </r>
   </si>
   <si>
@@ -1353,12 +1230,6 @@
     <t>Cooling Duct v2</t>
   </si>
   <si>
-    <t>Belt Guard</t>
-  </si>
-  <si>
-    <t>Belt Guard (Mirrored)</t>
-  </si>
-  <si>
     <t>Options</t>
   </si>
   <si>
@@ -1392,6 +1263,117 @@
   </si>
   <si>
     <t>Misc Wiring (not specified)</t>
+  </si>
+  <si>
+    <t>Bearing Holder with Pass Through</t>
+  </si>
+  <si>
+    <t>Belt Guard A</t>
+  </si>
+  <si>
+    <t>Belt Guard B</t>
+  </si>
+  <si>
+    <t>XY External Motor Mount</t>
+  </si>
+  <si>
+    <t>Outlet Switch Mount</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SKR 1.3 / 1.4 Controller </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>Mount</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>XY Side Carriage Za</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>ne V2.5 Rev2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>XY Side Carriage Zane V2.5 Rev2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (Mirrored)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Y (New) Endstop </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>Mount</t>
+    </r>
+  </si>
+  <si>
+    <t>X (NEW) Endstop Mount</t>
+  </si>
+  <si>
+    <t>Z (NEW) Endstop Mount</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Z Axis Bed Support </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>V2.5</t>
+    </r>
+  </si>
+  <si>
+    <t>Z Axis Shaft Mount A</t>
+  </si>
+  <si>
+    <t>Z Axis Shaft Mount B</t>
+  </si>
+  <si>
+    <r>
+      <t>Z Integrated Leadsc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>rew Motor Mount</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1531,7 +1513,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{AD2C3514-EDC6-42FF-9079-0FD21783A43F}" diskRevisions="1" revisionId="641" version="2">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{02BC1796-B453-4B04-8755-6519EBD860EB}" diskRevisions="1" revisionId="656" version="3">
   <header guid="{340CF866-0A5B-4738-BEFA-8F88CDCF6578}" dateTime="2020-07-10T21:00:06" maxSheetId="2" userName="eclsnowman" r:id="rId1">
     <sheetIdMap count="1">
       <sheetId val="1"/>
@@ -1572,6 +1554,11 @@
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
+  <header guid="{02BC1796-B453-4B04-8755-6519EBD860EB}" dateTime="2020-07-11T16:53:24" maxSheetId="2" userName="eclsnowman" r:id="rId9" minRId="642" maxRId="656">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -15150,8 +15137,345 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
+<file path=xl/revisions/revisionLog9.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="642" sId="1">
+    <oc r="B62" t="inlineStr">
+      <is>
+        <t>Bearing_Holder with Pass Through</t>
+      </is>
+    </oc>
+    <nc r="B62" t="inlineStr">
+      <is>
+        <t>Bearing Holder with Pass Through</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="643" sId="1">
+    <oc r="B80" t="inlineStr">
+      <is>
+        <t>Belt Guard</t>
+      </is>
+    </oc>
+    <nc r="B80" t="inlineStr">
+      <is>
+        <t>Belt Guard A</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="644" sId="1">
+    <oc r="B81" t="inlineStr">
+      <is>
+        <t>Belt Guard (Mirrored)</t>
+      </is>
+    </oc>
+    <nc r="B81" t="inlineStr">
+      <is>
+        <t>Belt Guard B</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="645" sId="1">
+    <oc r="B78" t="inlineStr">
+      <is>
+        <t>XY_External_Motor_Mount</t>
+      </is>
+    </oc>
+    <nc r="B78" t="inlineStr">
+      <is>
+        <t>XY External Motor Mount</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="646" sId="1">
+    <oc r="B99" t="inlineStr">
+      <is>
+        <t>Outlet_Switch_Mount</t>
+      </is>
+    </oc>
+    <nc r="B99" t="inlineStr">
+      <is>
+        <t>Outlet Switch Mount</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="647" sId="1">
+    <oc r="B93" t="inlineStr">
+      <is>
+        <r>
+          <t xml:space="preserve">SKR_1.3 / 1.4 Controller </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="8"/>
+            <rFont val="Century Gothic"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mount</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="B93" t="inlineStr">
+      <is>
+        <r>
+          <t xml:space="preserve">SKR 1.3 / 1.4 Controller </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="8"/>
+            <rFont val="Century Gothic"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mount</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="648" sId="1">
+    <oc r="B67" t="inlineStr">
+      <is>
+        <r>
+          <t>XY_Side_Carriage_Za</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="8"/>
+            <rFont val="Century Gothic"/>
+            <family val="2"/>
+          </rPr>
+          <t>ne_V2.5_Rev2</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="B67" t="inlineStr">
+      <is>
+        <r>
+          <t>XY Side Carriage Za</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="8"/>
+            <rFont val="Century Gothic"/>
+            <family val="2"/>
+          </rPr>
+          <t>ne V2.5 Rev2</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="649" sId="1">
+    <oc r="B72" t="inlineStr">
+      <is>
+        <r>
+          <t>XY_Side_Carriage_Zan</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="8"/>
+            <rFont val="Century Gothic"/>
+            <family val="2"/>
+          </rPr>
+          <t>e_V2.5_Rev2 (Mirrored)</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="B72" t="inlineStr">
+      <is>
+        <r>
+          <t>XY Side Carriage Zane V2.5 Rev2</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="8"/>
+            <rFont val="Century Gothic"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> (Mirrored)</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="650" sId="1">
+    <oc r="B88" t="inlineStr">
+      <is>
+        <r>
+          <t xml:space="preserve">Y (New) Endstop </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="8"/>
+            <rFont val="SWGDT"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="8"/>
+            <rFont val="Century Gothic"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mount</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="B88" t="inlineStr">
+      <is>
+        <r>
+          <t xml:space="preserve">Y (New) Endstop </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="8"/>
+            <rFont val="Century Gothic"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mount</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="651" sId="1">
+    <oc r="B85" t="inlineStr">
+      <is>
+        <t>X(NEW) Endstop Mount</t>
+      </is>
+    </oc>
+    <nc r="B85" t="inlineStr">
+      <is>
+        <t>X (NEW) Endstop Mount</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="652" sId="1">
+    <oc r="B101" t="inlineStr">
+      <is>
+        <t>Z(NEW) Endstop Mount</t>
+      </is>
+    </oc>
+    <nc r="B101" t="inlineStr">
+      <is>
+        <t>Z (NEW) Endstop Mount</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="653" sId="1">
+    <oc r="B21" t="inlineStr">
+      <is>
+        <r>
+          <t xml:space="preserve">Z_Axis_Bed_Support </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="8"/>
+            <rFont val="SWGDT"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="8"/>
+            <rFont val="Century Gothic"/>
+            <family val="2"/>
+          </rPr>
+          <t>V2.5</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="B21" t="inlineStr">
+      <is>
+        <r>
+          <t xml:space="preserve">Z Axis Bed Support </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="8"/>
+            <rFont val="Century Gothic"/>
+            <family val="2"/>
+          </rPr>
+          <t>V2.5</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="654" sId="1">
+    <oc r="B28" t="inlineStr">
+      <is>
+        <t>Z_Axis_Shaft_Mount_A</t>
+      </is>
+    </oc>
+    <nc r="B28" t="inlineStr">
+      <is>
+        <t>Z Axis Shaft Mount A</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="655" sId="1">
+    <oc r="B29" t="inlineStr">
+      <is>
+        <t>Z_Axis_Shaft_Mount_B</t>
+      </is>
+    </oc>
+    <nc r="B29" t="inlineStr">
+      <is>
+        <t>Z Axis Shaft Mount B</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="656" sId="1">
+    <oc r="B76" t="inlineStr">
+      <is>
+        <r>
+          <t>Z_Integrated_Leadsc</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="8"/>
+            <rFont val="Century Gothic"/>
+            <family val="2"/>
+          </rPr>
+          <t>rew_Motor_Mount</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="B76" t="inlineStr">
+      <is>
+        <r>
+          <t>Z Integrated Leadsc</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="8"/>
+            <rFont val="Century Gothic"/>
+            <family val="2"/>
+          </rPr>
+          <t>rew Motor Mount</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
+  <userInfo guid="{02BC1796-B453-4B04-8755-6519EBD860EB}" name="eclsnowman" id="-237690872" dateTime="2020-07-11T16:17:28"/>
+</users>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -15455,7 +15779,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15475,25 +15799,25 @@
         <v>1</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="27" x14ac:dyDescent="0.25">
@@ -15501,13 +15825,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E2" s="12">
         <v>0</v>
@@ -15516,7 +15840,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H2" s="13"/>
     </row>
@@ -15525,13 +15849,13 @@
         <v>8</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>183</v>
+        <v>315</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E3" s="12">
         <v>0</v>
@@ -15540,7 +15864,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H3" s="13"/>
     </row>
@@ -15549,13 +15873,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E4" s="12">
         <v>0</v>
@@ -15564,7 +15888,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H4" s="13"/>
     </row>
@@ -15573,13 +15897,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>191</v>
-      </c>
       <c r="D5" s="7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E5" s="12">
         <v>0</v>
@@ -15588,7 +15912,7 @@
         <v>0</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H5" s="13"/>
     </row>
@@ -15597,13 +15921,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E6" s="12">
         <v>0</v>
@@ -15612,7 +15936,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H6" s="13"/>
     </row>
@@ -15621,13 +15945,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E7" s="12">
         <v>0</v>
@@ -15636,7 +15960,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H7" s="13"/>
     </row>
@@ -15645,13 +15969,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E8" s="12">
         <v>0</v>
@@ -15660,7 +15984,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H8" s="13"/>
     </row>
@@ -15669,13 +15993,13 @@
         <v>1</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E9" s="12">
         <v>0</v>
@@ -15684,7 +16008,7 @@
         <v>0</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H9" s="13"/>
     </row>
@@ -15693,13 +16017,13 @@
         <v>1</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>319</v>
+        <v>306</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E10" s="12">
         <v>0</v>
@@ -15708,7 +16032,7 @@
         <v>0</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H10" s="13"/>
     </row>
@@ -15717,13 +16041,13 @@
         <v>1</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E11" s="12">
         <v>0</v>
@@ -15732,7 +16056,7 @@
         <v>0</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H11" s="13"/>
     </row>
@@ -15741,13 +16065,13 @@
         <v>2</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>217</v>
+        <v>318</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E12" s="12">
         <v>0</v>
@@ -15756,7 +16080,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H12" s="13"/>
     </row>
@@ -15765,13 +16089,13 @@
         <v>1</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E13" s="12">
         <v>0</v>
@@ -15780,7 +16104,7 @@
         <v>0</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H13" s="13"/>
     </row>
@@ -15789,13 +16113,13 @@
         <v>1</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>55</v>
+        <v>319</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E14" s="12">
         <v>0</v>
@@ -15804,7 +16128,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H14" s="13"/>
     </row>
@@ -15813,13 +16137,13 @@
         <v>1</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>294</v>
+        <v>320</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E15" s="12">
         <v>0</v>
@@ -15828,7 +16152,7 @@
         <v>0</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H15" s="13"/>
     </row>
@@ -15837,13 +16161,13 @@
         <v>1</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E16" s="12">
         <v>0</v>
@@ -15852,7 +16176,7 @@
         <v>0</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H16" s="13"/>
     </row>
@@ -15861,13 +16185,13 @@
         <v>1</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>48</v>
+        <v>324</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E17" s="12">
         <v>0</v>
@@ -15876,7 +16200,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H17" s="13"/>
     </row>
@@ -15885,13 +16209,13 @@
         <v>2</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>295</v>
+        <v>321</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E18" s="12">
         <v>0</v>
@@ -15900,7 +16224,7 @@
         <v>0</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H18" s="13"/>
     </row>
@@ -15909,13 +16233,13 @@
         <v>2</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>296</v>
+        <v>322</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E19" s="12">
         <v>0</v>
@@ -15924,7 +16248,7 @@
         <v>0</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H19" s="13"/>
     </row>
@@ -15933,13 +16257,13 @@
         <v>1</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>297</v>
+        <v>323</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E20" s="12">
         <v>0</v>
@@ -15948,7 +16272,7 @@
         <v>0</v>
       </c>
       <c r="G20" s="13" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H20" s="13"/>
     </row>
@@ -15957,13 +16281,13 @@
         <v>2</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>56</v>
+        <v>325</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E21" s="12">
         <v>0</v>
@@ -15972,7 +16296,7 @@
         <v>0</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H21" s="13"/>
     </row>
@@ -15981,13 +16305,13 @@
         <v>2</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>298</v>
+        <v>326</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E22" s="12">
         <v>0</v>
@@ -15996,7 +16320,7 @@
         <v>0</v>
       </c>
       <c r="G22" s="13" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H22" s="13"/>
     </row>
@@ -16005,13 +16329,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>18</v>
+        <v>327</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E23" s="12">
         <v>0</v>
@@ -16020,7 +16344,7 @@
         <v>0</v>
       </c>
       <c r="G23" s="13" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H23" s="13"/>
     </row>
@@ -16029,13 +16353,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>19</v>
+        <v>328</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E24" s="12">
         <v>0</v>
@@ -16044,7 +16368,7 @@
         <v>0</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H24" s="13"/>
     </row>
@@ -16053,13 +16377,13 @@
         <v>2</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>299</v>
+        <v>329</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E25" s="12">
         <v>0</v>
@@ -16068,7 +16392,7 @@
         <v>0</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H25" s="13"/>
     </row>
@@ -16077,13 +16401,13 @@
         <v>1</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>300</v>
+        <v>287</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>301</v>
+        <v>288</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E26" s="12">
         <f>25+22.5</f>
@@ -16094,10 +16418,10 @@
         <v>47.5</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -16105,13 +16429,13 @@
         <v>1</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E27" s="12">
         <f>19.98/4</f>
@@ -16121,7 +16445,7 @@
         <v>19.98</v>
       </c>
       <c r="G27" s="13" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="H27" s="13"/>
     </row>
@@ -16130,13 +16454,13 @@
         <v>2</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E28" s="12">
         <f>19.98/5</f>
@@ -16146,7 +16470,7 @@
         <v>19.98</v>
       </c>
       <c r="G28" s="13" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="H28" s="13"/>
     </row>
@@ -16155,13 +16479,13 @@
         <v>1</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E29" s="12">
         <v>6.99</v>
@@ -16171,7 +16495,7 @@
         <v>6.99</v>
       </c>
       <c r="G29" s="13" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="H29" s="13"/>
     </row>
@@ -16180,13 +16504,13 @@
         <v>4</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E30" s="12">
         <f>8.96/20</f>
@@ -16196,7 +16520,7 @@
         <v>8.9600000000000009</v>
       </c>
       <c r="G30" s="13" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="H30" s="13"/>
     </row>
@@ -16208,17 +16532,17 @@
         <v>13</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E31" s="12">
         <v>8.99</v>
       </c>
       <c r="F31" s="12"/>
       <c r="G31" s="13" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="H31" s="13"/>
     </row>
@@ -16227,13 +16551,13 @@
         <v>2</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>327</v>
+        <v>312</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>303</v>
+        <v>290</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E32" s="12">
         <v>26.78</v>
@@ -16243,7 +16567,7 @@
         <v>53.56</v>
       </c>
       <c r="G32" s="13" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="H32" s="13"/>
     </row>
@@ -16252,13 +16576,13 @@
         <v>1</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="E33" s="12">
         <v>73.45</v>
@@ -16268,10 +16592,10 @@
         <v>73.45</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="27" x14ac:dyDescent="0.25">
@@ -16279,13 +16603,13 @@
         <v>1</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="E34" s="12">
         <v>0</v>
@@ -16294,7 +16618,7 @@
         <v>0</v>
       </c>
       <c r="G34" s="13" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="H34" s="13"/>
     </row>
@@ -16303,13 +16627,13 @@
         <v>5</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="E35" s="12">
         <v>0</v>
@@ -16318,7 +16642,7 @@
         <v>0</v>
       </c>
       <c r="G35" s="13" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="H35" s="13"/>
     </row>
@@ -16327,13 +16651,13 @@
         <v>1</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="E36" s="12">
         <v>80</v>
@@ -16343,7 +16667,7 @@
         <v>80</v>
       </c>
       <c r="G36" s="13" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="H36" s="13"/>
     </row>
@@ -16352,13 +16676,13 @@
         <v>1</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E37" s="12">
         <v>0.51</v>
@@ -16368,7 +16692,7 @@
         <v>0.51</v>
       </c>
       <c r="G37" s="13" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="H37" s="13"/>
     </row>
@@ -16377,13 +16701,13 @@
         <v>1</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E38" s="12">
         <v>0.67</v>
@@ -16393,7 +16717,7 @@
         <v>0.67</v>
       </c>
       <c r="G38" s="13" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H38" s="13"/>
     </row>
@@ -16402,13 +16726,13 @@
         <v>10</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E39" s="12">
         <v>0.158</v>
@@ -16418,7 +16742,7 @@
         <v>1.58</v>
       </c>
       <c r="G39" s="13" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="H39" s="13"/>
     </row>
@@ -16427,13 +16751,13 @@
         <v>10</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E40" s="12">
         <v>0.184</v>
@@ -16443,7 +16767,7 @@
         <v>1.8399999999999999</v>
       </c>
       <c r="G40" s="13" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="H40" s="13"/>
     </row>
@@ -16455,10 +16779,10 @@
         <v>7</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="E41" s="12">
         <f>29.15/4</f>
@@ -16469,7 +16793,7 @@
         <v>7.2874999999999996</v>
       </c>
       <c r="G41" s="13" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="H41" s="13"/>
     </row>
@@ -16481,10 +16805,10 @@
         <v>5</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="E42" s="12">
         <v>29.15</v>
@@ -16494,7 +16818,7 @@
         <v>29.15</v>
       </c>
       <c r="G42" s="13" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="H42" s="13"/>
     </row>
@@ -16506,10 +16830,10 @@
         <v>9</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="E43" s="12">
         <f>29.15/4</f>
@@ -16520,7 +16844,7 @@
         <v>7.2874999999999996</v>
       </c>
       <c r="G43" s="13" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="H43" s="13"/>
     </row>
@@ -16532,10 +16856,10 @@
         <v>8</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="E44" s="12">
         <f>29.15/4</f>
@@ -16546,7 +16870,7 @@
         <v>7.2874999999999996</v>
       </c>
       <c r="G44" s="13" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="H44" s="13"/>
     </row>
@@ -16558,10 +16882,10 @@
         <v>6</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="E45" s="12">
         <f>29.15/4</f>
@@ -16572,7 +16896,7 @@
         <v>7.2874999999999996</v>
       </c>
       <c r="G45" s="13" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="H45" s="13"/>
     </row>
@@ -16581,13 +16905,13 @@
         <v>8</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="E46" s="12">
         <f>9.99/10</f>
@@ -16597,7 +16921,7 @@
         <v>9.99</v>
       </c>
       <c r="G46" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H46" s="13"/>
     </row>
@@ -16606,13 +16930,13 @@
         <v>1</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>304</v>
+        <v>291</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="E47" s="12">
         <v>42.72</v>
@@ -16622,10 +16946,10 @@
         <v>42.72</v>
       </c>
       <c r="G47" s="13" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="H47" s="13" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="27" x14ac:dyDescent="0.25">
@@ -16633,13 +16957,13 @@
         <v>8</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E48" s="12">
         <f>12.31/10</f>
@@ -16649,7 +16973,7 @@
         <v>12.31</v>
       </c>
       <c r="G48" s="13" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="H48" s="13"/>
     </row>
@@ -16658,13 +16982,13 @@
         <v>4</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E49" s="12">
         <v>4.76</v>
@@ -16674,7 +16998,7 @@
         <v>19.04</v>
       </c>
       <c r="G49" s="13" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="H49" s="13"/>
     </row>
@@ -16683,13 +17007,13 @@
         <v>8</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E50" s="12">
         <v>4.41</v>
@@ -16699,7 +17023,7 @@
         <v>35.28</v>
       </c>
       <c r="G50" s="13" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="H50" s="13"/>
     </row>
@@ -16708,13 +17032,13 @@
         <v>4</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E51" s="12">
         <f>5.96/3</f>
@@ -16725,7 +17049,7 @@
         <v>11.92</v>
       </c>
       <c r="G51" s="13" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="H51" s="13"/>
     </row>
@@ -16734,13 +17058,13 @@
         <v>4</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E52" s="12">
         <f>9.12/25</f>
@@ -16750,7 +17074,7 @@
         <v>9.1199999999999992</v>
       </c>
       <c r="G52" s="13" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="H52" s="13"/>
     </row>
@@ -16759,13 +17083,13 @@
         <v>4</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E53" s="12">
         <f>3.13/25</f>
@@ -16775,7 +17099,7 @@
         <v>3.13</v>
       </c>
       <c r="G53" s="13" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="H53" s="13"/>
     </row>
@@ -16784,13 +17108,13 @@
         <v>13</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E54" s="12">
         <f>16.69/100</f>
@@ -16800,7 +17124,7 @@
         <v>16.690000000000001</v>
       </c>
       <c r="G54" s="13" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="H54" s="13"/>
     </row>
@@ -16809,13 +17133,13 @@
         <v>4</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E55" s="12">
         <f>6.21/10</f>
@@ -16825,7 +17149,7 @@
         <v>6.21</v>
       </c>
       <c r="G55" s="13" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="H55" s="13"/>
     </row>
@@ -16834,13 +17158,13 @@
         <v>4</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E56" s="12">
         <f>9.73/10</f>
@@ -16850,7 +17174,7 @@
         <v>9.73</v>
       </c>
       <c r="G56" s="13" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="H56" s="13"/>
     </row>
@@ -16859,13 +17183,13 @@
         <v>16</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E57" s="12">
         <v>1.98</v>
@@ -16875,10 +17199,10 @@
         <v>31.68</v>
       </c>
       <c r="G57" s="13" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="H57" s="13" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="27" x14ac:dyDescent="0.25">
@@ -16886,13 +17210,13 @@
         <v>10</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E58" s="12">
         <v>7.93</v>
@@ -16902,7 +17226,7 @@
         <v>79.3</v>
       </c>
       <c r="G58" s="13" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="H58" s="13"/>
     </row>
@@ -16911,13 +17235,13 @@
         <v>4</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E59" s="12">
         <v>14.473000000000001</v>
@@ -16927,7 +17251,7 @@
         <v>57.892000000000003</v>
       </c>
       <c r="G59" s="13" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="H59" s="13"/>
     </row>
@@ -16936,13 +17260,13 @@
         <v>4</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E60" s="12">
         <v>1.97</v>
@@ -16952,10 +17276,10 @@
         <v>7.88</v>
       </c>
       <c r="G60" s="13" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="H60" s="13" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="27" x14ac:dyDescent="0.25">
@@ -16963,13 +17287,13 @@
         <v>2</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E61" s="12">
         <v>6.68</v>
@@ -16979,7 +17303,7 @@
         <v>13.36</v>
       </c>
       <c r="G61" s="13" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="H61" s="13"/>
     </row>
@@ -16988,13 +17312,13 @@
         <v>2</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E62" s="12">
         <v>3.27</v>
@@ -17004,7 +17328,7 @@
         <v>6.54</v>
       </c>
       <c r="G62" s="13" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="H62" s="13"/>
     </row>
@@ -17016,10 +17340,10 @@
         <v>17</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E63" s="12">
         <v>13.73</v>
@@ -17029,7 +17353,7 @@
         <v>27.46</v>
       </c>
       <c r="G63" s="13" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="H63" s="13"/>
     </row>
@@ -17038,13 +17362,13 @@
         <v>2</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E64" s="12">
         <v>13.73</v>
@@ -17054,7 +17378,7 @@
         <v>27.46</v>
       </c>
       <c r="G64" s="13" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="H64" s="13"/>
     </row>
@@ -17063,13 +17387,13 @@
         <v>2</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E65" s="12">
         <v>13.73</v>
@@ -17079,7 +17403,7 @@
         <v>27.46</v>
       </c>
       <c r="G65" s="13" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="H65" s="13"/>
     </row>
@@ -17088,13 +17412,13 @@
         <v>2</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E66" s="12">
         <v>13.41</v>
@@ -17104,7 +17428,7 @@
         <v>26.82</v>
       </c>
       <c r="G66" s="13" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="H66" s="13"/>
     </row>
@@ -17113,13 +17437,13 @@
         <v>1</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>305</v>
+        <v>292</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>306</v>
+        <v>293</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="E67" s="12">
         <v>25.71</v>
@@ -17129,10 +17453,10 @@
         <v>25.71</v>
       </c>
       <c r="G67" s="13" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="H67" s="13" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -17140,13 +17464,13 @@
         <v>1</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="E68" s="12">
         <v>30.52</v>
@@ -17156,10 +17480,10 @@
         <v>30.52</v>
       </c>
       <c r="G68" s="13" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="H68" s="13" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -17167,13 +17491,13 @@
         <v>2</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>316</v>
+        <v>303</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>317</v>
+        <v>304</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>315</v>
+        <v>302</v>
       </c>
       <c r="E69" s="12">
         <v>5</v>
@@ -17183,10 +17507,10 @@
         <v>10</v>
       </c>
       <c r="G69" s="14" t="s">
-        <v>314</v>
+        <v>301</v>
       </c>
       <c r="H69" s="14" t="s">
-        <v>318</v>
+        <v>305</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -17194,13 +17518,13 @@
         <v>1</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="E70" s="12">
         <v>34.979999999999997</v>
@@ -17210,10 +17534,10 @@
         <v>34.979999999999997</v>
       </c>
       <c r="G70" s="13" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="H70" s="13" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -17221,13 +17545,13 @@
         <v>1</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="E71" s="12">
         <v>10.99</v>
@@ -17237,10 +17561,10 @@
         <v>10.99</v>
       </c>
       <c r="G71" s="13" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="H71" s="13" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -17248,13 +17572,13 @@
         <v>1</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="E72" s="12">
         <v>61.9</v>
@@ -17264,10 +17588,10 @@
         <v>61.9</v>
       </c>
       <c r="G72" s="13" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="H72" s="13" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -17275,13 +17599,13 @@
         <v>10</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D73" s="7" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E73" s="12">
         <v>1.6</v>
@@ -17291,10 +17615,10 @@
         <v>16</v>
       </c>
       <c r="G73" s="13" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="H73" s="13" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -17305,10 +17629,10 @@
         <v>3</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D74" s="7" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E74" s="12">
         <f>7.5/100</f>
@@ -17319,10 +17643,10 @@
         <v>15</v>
       </c>
       <c r="G74" s="13" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="H74" s="13" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -17330,13 +17654,13 @@
         <v>4</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>309</v>
+        <v>296</v>
       </c>
       <c r="D75" s="7" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E75" s="12">
         <f>(0.85/5)*6</f>
@@ -17346,10 +17670,10 @@
         <v>6</v>
       </c>
       <c r="G75" s="13" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="H75" s="13" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="27" x14ac:dyDescent="0.25">
@@ -17357,13 +17681,13 @@
         <v>2</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="D76" s="7" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E76" s="12">
         <v>0.35</v>
@@ -17373,10 +17697,10 @@
         <v>0.7</v>
       </c>
       <c r="G76" s="13" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="H76" s="13" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="27" x14ac:dyDescent="0.25">
@@ -17387,10 +17711,10 @@
         <v>12</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="D77" s="7" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E77" s="12">
         <v>1.5</v>
@@ -17400,10 +17724,10 @@
         <v>3</v>
       </c>
       <c r="G77" s="13" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="H77" s="13" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -17411,13 +17735,13 @@
         <v>1</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="D78" s="7" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="E78" s="12">
         <v>6.6</v>
@@ -17427,10 +17751,10 @@
         <v>6.6</v>
       </c>
       <c r="G78" s="13" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="H78" s="13" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -17438,13 +17762,13 @@
         <v>2</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D79" s="7" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E79" s="12">
         <f>0.62/25</f>
@@ -17454,7 +17778,7 @@
         <v>0.62</v>
       </c>
       <c r="G79" s="13" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="H79" s="13"/>
     </row>
@@ -17463,13 +17787,13 @@
         <v>4</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D80" s="7" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E80" s="12">
         <f>0.49/25</f>
@@ -17479,7 +17803,7 @@
         <v>0.49</v>
       </c>
       <c r="G80" s="13" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="H80" s="13"/>
     </row>
@@ -17488,13 +17812,13 @@
         <v>10</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D81" s="7" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E81" s="12">
         <f>0.64/25</f>
@@ -17504,7 +17828,7 @@
         <v>0.64</v>
       </c>
       <c r="G81" s="13" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H81" s="13"/>
     </row>
@@ -17513,13 +17837,13 @@
         <v>16</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D82" s="7" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E82" s="12">
         <f>0.67/25</f>
@@ -17529,7 +17853,7 @@
         <v>0.67</v>
       </c>
       <c r="G82" s="13" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="H82" s="13"/>
     </row>
@@ -17538,13 +17862,13 @@
         <v>8</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D83" s="7" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E83" s="12">
         <f>0.83/25</f>
@@ -17554,7 +17878,7 @@
         <v>0.83</v>
       </c>
       <c r="G83" s="13" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="H83" s="13"/>
     </row>
@@ -17563,13 +17887,13 @@
         <v>2</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D84" s="7" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E84" s="12">
         <f>0.65/25</f>
@@ -17579,7 +17903,7 @@
         <v>0.65</v>
       </c>
       <c r="G84" s="13" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="H84" s="13"/>
     </row>
@@ -17591,10 +17915,10 @@
         <v>16</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D85" s="7" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E85" s="12">
         <f>0.62/25</f>
@@ -17604,7 +17928,7 @@
         <v>0.62</v>
       </c>
       <c r="G85" s="13" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="H85" s="13"/>
     </row>
@@ -17613,13 +17937,13 @@
         <v>8</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D86" s="7" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E86" s="12">
         <f>0.87/25</f>
@@ -17629,7 +17953,7 @@
         <v>0.87</v>
       </c>
       <c r="G86" s="13" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="H86" s="13"/>
     </row>
@@ -17641,10 +17965,10 @@
         <v>10</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D87" s="7" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E87" s="12">
         <f>1/25</f>
@@ -17654,7 +17978,7 @@
         <v>1</v>
       </c>
       <c r="G87" s="13" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="H87" s="13"/>
     </row>
@@ -17663,13 +17987,13 @@
         <v>1</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D88" s="7" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E88" s="12">
         <f>1.04/25</f>
@@ -17679,7 +18003,7 @@
         <v>1.04</v>
       </c>
       <c r="G88" s="13" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H88" s="13"/>
     </row>
@@ -17688,13 +18012,13 @@
         <v>2</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D89" s="7" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E89" s="12">
         <f>0.72/12</f>
@@ -17704,7 +18028,7 @@
         <v>0.72</v>
       </c>
       <c r="G89" s="13" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H89" s="13"/>
     </row>
@@ -17713,13 +18037,13 @@
         <v>4</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D90" s="7" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E90" s="12">
         <f>0.58/25</f>
@@ -17729,7 +18053,7 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="G90" s="13" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="H90" s="13"/>
     </row>
@@ -17738,13 +18062,13 @@
         <v>2</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D91" s="7" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E91" s="12">
         <f>0.93/25</f>
@@ -17754,7 +18078,7 @@
         <v>0.93</v>
       </c>
       <c r="G91" s="13" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="H91" s="13"/>
     </row>
@@ -17766,10 +18090,10 @@
         <v>2</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D92" s="7" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E92" s="12">
         <f>0.56/12</f>
@@ -17780,7 +18104,7 @@
         <v>6.16</v>
       </c>
       <c r="G92" s="13" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="H92" s="13"/>
     </row>
@@ -17789,13 +18113,13 @@
         <v>26</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D93" s="7" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E93" s="12">
         <f>0.66/12</f>
@@ -17806,7 +18130,7 @@
         <v>1.98</v>
       </c>
       <c r="G93" s="13" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="H93" s="13"/>
     </row>
@@ -17818,10 +18142,10 @@
         <v>15</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D94" s="7" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E94" s="12">
         <f>0.67/12</f>
@@ -17831,7 +18155,7 @@
         <v>0.67</v>
       </c>
       <c r="G94" s="13" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="H94" s="13"/>
     </row>
@@ -17843,10 +18167,10 @@
         <v>4</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D95" s="7" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E95" s="12">
         <f>0.67/12</f>
@@ -17856,7 +18180,7 @@
         <v>0.67</v>
       </c>
       <c r="G95" s="13" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="H95" s="13"/>
     </row>
@@ -17865,13 +18189,13 @@
         <v>8</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>312</v>
+        <v>299</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>313</v>
+        <v>300</v>
       </c>
       <c r="D96" s="7" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E96" s="12">
         <f>0.69/12</f>
@@ -17881,7 +18205,7 @@
         <v>0.69</v>
       </c>
       <c r="G96" s="13" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="H96" s="13"/>
     </row>
@@ -17890,13 +18214,13 @@
         <v>4</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D97" s="7" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E97" s="12">
         <f>0.84/12</f>
@@ -17906,7 +18230,7 @@
         <v>0.84</v>
       </c>
       <c r="G97" s="13" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="H97" s="13"/>
     </row>
@@ -17915,13 +18239,13 @@
         <v>6</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D98" s="7" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E98" s="12">
         <f>0.56/12</f>
@@ -17931,7 +18255,7 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="G98" s="13" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="H98" s="13"/>
     </row>
@@ -17940,13 +18264,13 @@
         <v>8</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="D99" s="7" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E99" s="12">
         <f>0.15/25</f>
@@ -17956,7 +18280,7 @@
         <v>0.15</v>
       </c>
       <c r="G99" s="13" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="H99" s="13"/>
     </row>
@@ -17968,10 +18292,10 @@
         <v>11</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="D100" s="7" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E100" s="12">
         <f>0.41/25</f>
@@ -17981,7 +18305,7 @@
         <v>0.41</v>
       </c>
       <c r="G100" s="13" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="H100" s="13"/>
     </row>
@@ -17990,13 +18314,13 @@
         <v>2</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="D101" s="7" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E101" s="12">
         <f>0.66/25</f>
@@ -18006,7 +18330,7 @@
         <v>0.66</v>
       </c>
       <c r="G101" s="13" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="H101" s="13"/>
     </row>
@@ -18015,13 +18339,13 @@
         <v>4</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="D102" s="7" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E102" s="12">
         <f>0.64/25</f>
@@ -18031,7 +18355,7 @@
         <v>0.64</v>
       </c>
       <c r="G102" s="13" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="H102" s="13"/>
     </row>
@@ -18040,13 +18364,13 @@
         <v>8</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="D103" s="7" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E103" s="12">
         <f>0.2/25</f>
@@ -18056,7 +18380,7 @@
         <v>0.2</v>
       </c>
       <c r="G103" s="13" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="H103" s="13"/>
     </row>
@@ -18068,10 +18392,10 @@
         <v>14</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="D104" s="7" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E104" s="12">
         <f>0.56/25</f>
@@ -18081,7 +18405,7 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="G104" s="13" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="H104" s="13"/>
     </row>
@@ -18090,13 +18414,13 @@
         <v>12</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D105" s="7" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E105" s="12">
         <f>0.69/25</f>
@@ -18106,13 +18430,13 @@
         <v>0.69</v>
       </c>
       <c r="G105" s="13" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="H105" s="13"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E107" s="2" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="F107" s="2">
         <f>SUM(F2:F105)</f>
@@ -18121,7 +18445,7 @@
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B108" s="7" t="s">
-        <v>322</v>
+        <v>307</v>
       </c>
     </row>
     <row r="109" spans="1:8" ht="27" x14ac:dyDescent="0.25">
@@ -18129,13 +18453,13 @@
         <v>1</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>326</v>
+        <v>311</v>
       </c>
       <c r="C109" s="11" t="s">
-        <v>323</v>
+        <v>308</v>
       </c>
       <c r="D109" s="10" t="s">
-        <v>325</v>
+        <v>310</v>
       </c>
       <c r="E109" s="1">
         <v>60.12</v>
@@ -18145,17 +18469,17 @@
         <v>60.12</v>
       </c>
       <c r="G109" t="s">
-        <v>324</v>
+        <v>309</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B111" s="10" t="s">
-        <v>328</v>
+        <v>313</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B112" s="10" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated BOMs and Drawings, John Phan noticed some errors
Updated Prints and BOM with corrections and additions notice by someone building the printer (John Phan).
</commit_message>
<xml_diff>
--- a/BOM/ES25 BOM.xlsx
+++ b/BOM/ES25 BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Documents\04 - Github\Eustathios-Spider-V2.5\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{DA344A2D-159A-4B78-9CD1-03C0F865D620}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{E4173DD2-13DF-4A24-B2A7-A66C05430C5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="342">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -1386,6 +1386,30 @@
   </si>
   <si>
     <t>Misc Vitamines and Other Parts</t>
+  </si>
+  <si>
+    <t>X and Y Motors</t>
+  </si>
+  <si>
+    <t>Nema17 60mm Drive Motors</t>
+  </si>
+  <si>
+    <t>https://www.robotdigg.com/product/29/Nema17-60mm-1.5A-high-torque-stepper-motor</t>
+  </si>
+  <si>
+    <t>https://www.printedsolid.com/products/ldo-nema-17-motor-supermac-ldo-42sth60-2004ac</t>
+  </si>
+  <si>
+    <t>Change Log:</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>Updated 07-14-20, User noted I was missing X/Y Motors. I added them to the sheet</t>
+  </si>
+  <si>
+    <t>https://www.trimcraftaviationrc.com/index.php?route=product/product&amp;path=72&amp;product_id=455</t>
   </si>
 </sst>
 </file>
@@ -1486,7 +1510,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1528,6 +1552,9 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1546,7 +1573,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{389F9543-221C-4381-A4EE-901DB4B59CE2}" diskRevisions="1" revisionId="690" version="4">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{4F55D34C-EB41-47DF-A59F-E8F9776E9C20}" diskRevisions="1" revisionId="715" version="6">
   <header guid="{340CF866-0A5B-4738-BEFA-8F88CDCF6578}" dateTime="2020-07-10T21:00:06" maxSheetId="2" userName="eclsnowman" r:id="rId1">
     <sheetIdMap count="1">
       <sheetId val="1"/>
@@ -1597,6 +1624,16 @@
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
+  <header guid="{EC441586-1321-4951-8AC7-2D5D2F740C7D}" dateTime="2020-07-14T11:10:50" maxSheetId="2" userName="eclsnowman" r:id="rId11" minRId="691" maxRId="709">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{4F55D34C-EB41-47DF-A59F-E8F9776E9C20}" dateTime="2020-07-14T11:21:47" maxSheetId="2" userName="eclsnowman" r:id="rId12" minRId="711" maxRId="715">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -2379,6 +2416,255 @@
       </font>
     </dxf>
   </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog11.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="691" sId="1" ref="A78:XFD78" action="insertRow"/>
+  <rcc rId="692" sId="1">
+    <nc r="A78">
+      <v>1</v>
+    </nc>
+  </rcc>
+  <rcc rId="693" sId="1">
+    <nc r="B78" t="inlineStr">
+      <is>
+        <t>Extruder Motor</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="694" sId="1">
+    <nc r="C78" t="inlineStr">
+      <is>
+        <t>Nema17 Extruder Stepper Motor for BMG</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="695" sId="1">
+    <nc r="D78" t="inlineStr">
+      <is>
+        <t>Robotdigg or Printed Solid</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="696" sId="1" numFmtId="11">
+    <nc r="E78">
+      <v>6.6</v>
+    </nc>
+  </rcc>
+  <rcc rId="697" sId="1">
+    <nc r="F78">
+      <f>E78*A78</f>
+    </nc>
+  </rcc>
+  <rcc rId="698" sId="1">
+    <nc r="G78" t="inlineStr">
+      <is>
+        <t>https://www.robotdigg.com/product/7/NEMA17-40mm-long-17hs3001-20b-Stepper-Motor</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="699" sId="1">
+    <nc r="H78" t="inlineStr">
+      <is>
+        <t>https://www.printedsolid.com/collections/motors/products/ldo-nema-17-motor-high-temp-180c-ldo-42sth40-1004ah</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="700" sId="1">
+    <oc r="B79" t="inlineStr">
+      <is>
+        <t>Extruder Motor</t>
+      </is>
+    </oc>
+    <nc r="B79" t="inlineStr">
+      <is>
+        <t>X and Y Motors</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="701" sId="1">
+    <oc r="C79" t="inlineStr">
+      <is>
+        <t>Nema17 Extruder Stepper Motor for BMG</t>
+      </is>
+    </oc>
+    <nc r="C79" t="inlineStr">
+      <is>
+        <t>Nema17 60mm Drive Motors</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="702" sId="1">
+    <oc r="A79">
+      <v>1</v>
+    </oc>
+    <nc r="A79">
+      <v>2</v>
+    </nc>
+  </rcc>
+  <rcc rId="703" sId="1">
+    <oc r="G79" t="inlineStr">
+      <is>
+        <t>https://www.robotdigg.com/product/7/NEMA17-40mm-long-17hs3001-20b-Stepper-Motor</t>
+      </is>
+    </oc>
+    <nc r="G79" t="inlineStr">
+      <is>
+        <t>https://www.robotdigg.com/product/29/Nema17-60mm-1.5A-high-torque-stepper-motor</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="704" sId="1" numFmtId="11">
+    <oc r="E79">
+      <v>6.6</v>
+    </oc>
+    <nc r="E79">
+      <v>10.9</v>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="H79" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom"/>
+    </dxf>
+  </rfmt>
+  <rcc rId="705" sId="1" xfDxf="1" dxf="1">
+    <oc r="H79" t="inlineStr">
+      <is>
+        <t>https://www.printedsolid.com/collections/motors/products/ldo-nema-17-motor-high-temp-180c-ldo-42sth40-1004ah</t>
+      </is>
+    </oc>
+    <nc r="H79" t="inlineStr">
+      <is>
+        <t>https://www.printedsolid.com/products/ldo-nema-17-motor-supermac-ldo-42sth60-2004ac</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="B116">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rm rId="706" sheetId="1" source="B116" destination="B117" sourceSheetId="1"/>
+  <rcc rId="707" sId="1">
+    <nc r="B116" t="inlineStr">
+      <is>
+        <t>Change Log:</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="B116">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="B116" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <u/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="B116" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="708" sId="1">
+    <nc r="A117" t="inlineStr">
+      <is>
+        <t>R1</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="A117">
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+  </rfmt>
+  <rcc rId="709" sId="1">
+    <nc r="B117" t="inlineStr">
+      <is>
+        <t>Updated 07-14-20, User noted I was missing X/Y Motors. I added them to the sheet</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="B117">
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+  </rfmt>
+  <rcv guid="{558925EA-5CF7-4433-B1B3-D7D45C0B5112}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_558925EA_5CF7_4433_B1B3_D7D45C0B5112_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Sheet1!$A$1:$H$1</formula>
+    <oldFormula>Sheet1!$A$1:$H$1</oldFormula>
+  </rdn>
+  <rcv guid="{558925EA-5CF7-4433-B1B3-D7D45C0B5112}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog12.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="711" sId="1">
+    <nc r="H38" t="inlineStr">
+      <is>
+        <t>https://www.mcmaster.com/94545A225/</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="712" sId="1">
+    <oc r="G38" t="inlineStr">
+      <is>
+        <t>https://www.mcmaster.com/94545A225/</t>
+      </is>
+    </oc>
+    <nc r="G38" t="inlineStr">
+      <is>
+        <t>https://www.trimcraftaviationrc.com/index.php?route=product/product&amp;path=72&amp;product_id=455</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="713" sId="1">
+    <oc r="E38">
+      <f>6.21/10</f>
+    </oc>
+    <nc r="E38">
+      <f>0.44/4</f>
+    </nc>
+  </rcc>
+  <rcc rId="714" sId="1" odxf="1" dxf="1">
+    <oc r="F38">
+      <v>6.21</v>
+    </oc>
+    <nc r="F38">
+      <f>E38*A38</f>
+    </nc>
+    <ndxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="715" sId="1">
+    <oc r="D38" t="inlineStr">
+      <is>
+        <t>McMaster Carr</t>
+      </is>
+    </oc>
+    <nc r="D38" t="inlineStr">
+      <is>
+        <t>Trimcraft Aviation RC</t>
+      </is>
+    </nc>
+  </rcc>
 </revisions>
 </file>
 
@@ -16589,11 +16875,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H113"/>
+  <dimension ref="A1:H117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16634,15 +16920,15 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>282</v>
+        <v>313</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>133</v>
+        <v>177</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>132</v>
@@ -16660,13 +16946,13 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>313</v>
+        <v>26</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>132</v>
@@ -16687,7 +16973,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>26</v>
+        <v>178</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>184</v>
@@ -16708,13 +16994,13 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>178</v>
+        <v>314</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>132</v>
@@ -16735,10 +17021,10 @@
         <v>1</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>132</v>
@@ -16759,10 +17045,10 @@
         <v>1</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>315</v>
+        <v>44</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>132</v>
@@ -16783,10 +17069,10 @@
         <v>1</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>44</v>
+        <v>283</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>132</v>
@@ -16807,10 +17093,10 @@
         <v>1</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>283</v>
+        <v>305</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>132</v>
@@ -16831,10 +17117,10 @@
         <v>1</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>305</v>
+        <v>285</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>204</v>
+        <v>232</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>132</v>
@@ -16850,15 +17136,15 @@
       </c>
       <c r="H10" s="10"/>
     </row>
-    <row r="11" spans="1:8" ht="27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>1</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>284</v>
+        <v>317</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>205</v>
+        <v>255</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>132</v>
@@ -16876,13 +17162,13 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>210</v>
+        <v>268</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>132</v>
@@ -16898,15 +17184,15 @@
       </c>
       <c r="H12" s="10"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="27" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>1</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>285</v>
+        <v>27</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>232</v>
+        <v>269</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>132</v>
@@ -16922,15 +17208,15 @@
       </c>
       <c r="H13" s="10"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="27" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>1</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>317</v>
+        <v>284</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>255</v>
+        <v>205</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>132</v>
@@ -16946,15 +17232,15 @@
       </c>
       <c r="H14" s="10"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="27" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>1</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>318</v>
+        <v>282</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>268</v>
+        <v>133</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>132</v>
@@ -16970,15 +17256,15 @@
       </c>
       <c r="H15" s="10"/>
     </row>
-    <row r="16" spans="1:8" ht="27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>1</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>27</v>
+        <v>322</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>132</v>
@@ -16994,15 +17280,15 @@
       </c>
       <c r="H16" s="10"/>
     </row>
-    <row r="17" spans="1:8" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>274</v>
+        <v>210</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>132</v>
@@ -17477,7 +17763,7 @@
         <v>80</v>
       </c>
       <c r="F36" s="9">
-        <f t="shared" ref="F36:F45" si="0">E36*A36</f>
+        <f>E36*A36</f>
         <v>80</v>
       </c>
       <c r="G36" s="10" t="s">
@@ -17502,7 +17788,7 @@
         <v>0.51</v>
       </c>
       <c r="F37" s="9">
-        <f t="shared" si="0"/>
+        <f>E37*A37</f>
         <v>0.51</v>
       </c>
       <c r="G37" s="10" t="s">
@@ -17527,7 +17813,7 @@
         <v>0.67</v>
       </c>
       <c r="F38" s="9">
-        <f t="shared" si="0"/>
+        <f>E38*A38</f>
         <v>0.67</v>
       </c>
       <c r="G38" s="10" t="s">
@@ -17552,7 +17838,7 @@
         <v>0.158</v>
       </c>
       <c r="F39" s="9">
-        <f t="shared" si="0"/>
+        <f>E39*A39</f>
         <v>1.58</v>
       </c>
       <c r="G39" s="10" t="s">
@@ -17577,7 +17863,7 @@
         <v>0.184</v>
       </c>
       <c r="F40" s="9">
-        <f t="shared" si="0"/>
+        <f>E40*A40</f>
         <v>1.8399999999999999</v>
       </c>
       <c r="G40" s="10" t="s">
@@ -17603,7 +17889,7 @@
         <v>7.2874999999999996</v>
       </c>
       <c r="F41" s="9">
-        <f t="shared" si="0"/>
+        <f>E41*A41</f>
         <v>7.2874999999999996</v>
       </c>
       <c r="G41" s="10" t="s">
@@ -17628,7 +17914,7 @@
         <v>29.15</v>
       </c>
       <c r="F42" s="9">
-        <f t="shared" si="0"/>
+        <f>E42*A42</f>
         <v>29.15</v>
       </c>
       <c r="G42" s="10" t="s">
@@ -17654,7 +17940,7 @@
         <v>7.2874999999999996</v>
       </c>
       <c r="F43" s="9">
-        <f t="shared" si="0"/>
+        <f>E43*A43</f>
         <v>7.2874999999999996</v>
       </c>
       <c r="G43" s="10" t="s">
@@ -17680,7 +17966,7 @@
         <v>7.2874999999999996</v>
       </c>
       <c r="F44" s="9">
-        <f t="shared" si="0"/>
+        <f>E44*A44</f>
         <v>7.2874999999999996</v>
       </c>
       <c r="G44" s="10" t="s">
@@ -17706,7 +17992,7 @@
         <v>7.2874999999999996</v>
       </c>
       <c r="F45" s="9">
-        <f t="shared" si="0"/>
+        <f>E45*A45</f>
         <v>7.2874999999999996</v>
       </c>
       <c r="G45" s="10" t="s">
@@ -17768,102 +18054,102 @@
     </row>
     <row r="48" spans="1:8" ht="27" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
-        <v>8</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>78</v>
+        <v>4</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>79</v>
       </c>
       <c r="E48" s="9">
-        <f>12.31/10</f>
-        <v>1.2310000000000001</v>
+        <v>4.76</v>
       </c>
       <c r="F48" s="9">
-        <v>12.31</v>
+        <f>E48*A48</f>
+        <v>19.04</v>
       </c>
       <c r="G48" s="10" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="H48" s="10"/>
     </row>
     <row r="49" spans="1:8" ht="27" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>79</v>
       </c>
       <c r="E49" s="9">
-        <v>4.76</v>
+        <v>4.41</v>
       </c>
       <c r="F49" s="9">
         <f>E49*A49</f>
-        <v>19.04</v>
+        <v>35.28</v>
       </c>
       <c r="G49" s="10" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H49" s="10"/>
     </row>
     <row r="50" spans="1:8" ht="27" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>84</v>
+        <v>159</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>79</v>
       </c>
       <c r="E50" s="9">
-        <v>4.41</v>
+        <f>5.96/3</f>
+        <v>1.9866666666666666</v>
       </c>
       <c r="F50" s="9">
-        <f>E50*A50</f>
-        <v>35.28</v>
+        <f>5.96*2</f>
+        <v>11.92</v>
       </c>
       <c r="G50" s="10" t="s">
-        <v>85</v>
+        <v>157</v>
       </c>
       <c r="H50" s="10"/>
     </row>
     <row r="51" spans="1:8" ht="27" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
-        <v>4</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>21</v>
+        <v>8</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>78</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>159</v>
+        <v>77</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>79</v>
       </c>
       <c r="E51" s="9">
-        <f>5.96/3</f>
-        <v>1.9866666666666666</v>
+        <f>12.31/10</f>
+        <v>1.2310000000000001</v>
       </c>
       <c r="F51" s="9">
-        <f>5.96*2</f>
-        <v>11.92</v>
+        <v>12.31</v>
       </c>
       <c r="G51" s="10" t="s">
-        <v>157</v>
+        <v>76</v>
       </c>
       <c r="H51" s="10"/>
     </row>
@@ -17947,202 +18233,202 @@
         <v>4</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>22</v>
+        <v>167</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>79</v>
       </c>
       <c r="E55" s="9">
-        <f>6.21/10</f>
-        <v>0.621</v>
+        <f>9.73/10</f>
+        <v>0.97300000000000009</v>
       </c>
       <c r="F55" s="9">
-        <v>6.21</v>
+        <v>9.73</v>
       </c>
       <c r="G55" s="10" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="H55" s="10"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
+        <v>16</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E56" s="9">
+        <v>1.98</v>
+      </c>
+      <c r="F56" s="9">
+        <f>E56*A56</f>
+        <v>31.68</v>
+      </c>
+      <c r="G56" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="H56" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="27" x14ac:dyDescent="0.25">
+      <c r="A57" s="3">
         <v>4</v>
       </c>
-      <c r="B56" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E56" s="9">
-        <f>9.73/10</f>
-        <v>0.97300000000000009</v>
-      </c>
-      <c r="F56" s="9">
-        <v>9.73</v>
-      </c>
-      <c r="G56" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="H56" s="10"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="3">
-        <v>16</v>
-      </c>
       <c r="B57" s="4" t="s">
-        <v>87</v>
+        <v>223</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>88</v>
+        <v>222</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>89</v>
       </c>
       <c r="E57" s="9">
-        <v>1.98</v>
+        <v>1.97</v>
       </c>
       <c r="F57" s="9">
         <f>E57*A57</f>
-        <v>31.68</v>
+        <v>7.88</v>
       </c>
       <c r="G57" s="10" t="s">
-        <v>94</v>
+        <v>224</v>
       </c>
       <c r="H57" s="10" t="s">
-        <v>86</v>
+        <v>225</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="27" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>90</v>
+        <v>226</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>89</v>
       </c>
       <c r="E58" s="9">
-        <v>7.93</v>
+        <v>6.68</v>
       </c>
       <c r="F58" s="9">
-        <f>E58*A58</f>
-        <v>79.3</v>
+        <f>A58*E58</f>
+        <v>13.36</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>93</v>
+        <v>228</v>
       </c>
       <c r="H58" s="10"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>91</v>
+        <v>229</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>95</v>
+        <v>230</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>89</v>
       </c>
       <c r="E59" s="9">
-        <v>14.473000000000001</v>
+        <v>3.27</v>
       </c>
       <c r="F59" s="9">
-        <f>E59*A59</f>
-        <v>57.892000000000003</v>
+        <f>A59*E59</f>
+        <v>6.54</v>
       </c>
       <c r="G59" s="10" t="s">
-        <v>92</v>
+        <v>231</v>
       </c>
       <c r="H59" s="10"/>
     </row>
     <row r="60" spans="1:8" ht="27" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>223</v>
+        <v>90</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>89</v>
       </c>
       <c r="E60" s="9">
-        <v>1.97</v>
+        <v>7.93</v>
       </c>
       <c r="F60" s="9">
         <f>E60*A60</f>
-        <v>7.88</v>
+        <v>79.3</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="H60" s="10" t="s">
-        <v>225</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="H60" s="10"/>
     </row>
-    <row r="61" spans="1:8" ht="27" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>226</v>
+        <v>91</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>227</v>
+        <v>95</v>
       </c>
       <c r="D61" s="4" t="s">
         <v>89</v>
       </c>
       <c r="E61" s="9">
-        <v>6.68</v>
+        <v>14.473000000000001</v>
       </c>
       <c r="F61" s="9">
-        <f>A61*E61</f>
-        <v>13.36</v>
+        <f>E61*A61</f>
+        <v>57.892000000000003</v>
       </c>
       <c r="G61" s="10" t="s">
-        <v>228</v>
+        <v>92</v>
       </c>
       <c r="H61" s="10"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="27" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>2</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>229</v>
+        <v>17</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>230</v>
+        <v>267</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>89</v>
       </c>
       <c r="E62" s="9">
-        <v>3.27</v>
+        <v>13.73</v>
       </c>
       <c r="F62" s="9">
-        <f>A62*E62</f>
-        <v>6.54</v>
+        <f>E62*A62</f>
+        <v>27.46</v>
       </c>
       <c r="G62" s="10" t="s">
-        <v>231</v>
+        <v>260</v>
       </c>
       <c r="H62" s="10"/>
     </row>
@@ -18151,10 +18437,10 @@
         <v>2</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>89</v>
@@ -18163,11 +18449,11 @@
         <v>13.73</v>
       </c>
       <c r="F63" s="9">
-        <f t="shared" ref="F63:F69" si="1">E63*A63</f>
+        <f>E63*A63</f>
         <v>27.46</v>
       </c>
       <c r="G63" s="10" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="H63" s="10"/>
     </row>
@@ -18176,10 +18462,10 @@
         <v>2</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>89</v>
@@ -18188,11 +18474,11 @@
         <v>13.73</v>
       </c>
       <c r="F64" s="9">
-        <f t="shared" si="1"/>
+        <f>E64*A64</f>
         <v>27.46</v>
       </c>
       <c r="G64" s="10" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="H64" s="10"/>
     </row>
@@ -18201,130 +18487,132 @@
         <v>2</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>89</v>
       </c>
       <c r="E65" s="9">
-        <v>13.73</v>
+        <v>13.41</v>
       </c>
       <c r="F65" s="9">
-        <f t="shared" si="1"/>
-        <v>27.46</v>
+        <f>E65*A65</f>
+        <v>26.82</v>
       </c>
       <c r="G65" s="10" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="H65" s="10"/>
     </row>
-    <row r="66" spans="1:8" ht="27" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>43</v>
+        <v>291</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>264</v>
+        <v>292</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>89</v>
+        <v>252</v>
       </c>
       <c r="E66" s="9">
-        <v>13.41</v>
+        <v>25.71</v>
       </c>
       <c r="F66" s="9">
-        <f t="shared" si="1"/>
-        <v>26.82</v>
+        <f>E66*A66</f>
+        <v>25.71</v>
       </c>
       <c r="G66" s="10" t="s">
-        <v>263</v>
-      </c>
-      <c r="H66" s="10"/>
+        <v>251</v>
+      </c>
+      <c r="H66" s="10" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>1</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>291</v>
+        <v>211</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>292</v>
+        <v>212</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>252</v>
+        <v>213</v>
       </c>
       <c r="E67" s="9">
-        <v>25.71</v>
+        <v>30.52</v>
       </c>
       <c r="F67" s="9">
-        <f t="shared" si="1"/>
-        <v>25.71</v>
+        <f>E67*A67</f>
+        <v>30.52</v>
       </c>
       <c r="G67" s="10" t="s">
-        <v>251</v>
+        <v>214</v>
       </c>
       <c r="H67" s="10" t="s">
-        <v>250</v>
+        <v>215</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>211</v>
+        <v>302</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>212</v>
+        <v>303</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>213</v>
+        <v>301</v>
       </c>
       <c r="E68" s="9">
-        <v>30.52</v>
+        <v>5</v>
       </c>
       <c r="F68" s="9">
-        <f t="shared" si="1"/>
-        <v>30.52</v>
-      </c>
-      <c r="G68" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="H68" s="10" t="s">
-        <v>215</v>
+        <f>E68*A68</f>
+        <v>10</v>
+      </c>
+      <c r="G68" s="11" t="s">
+        <v>300</v>
+      </c>
+      <c r="H68" s="11" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>302</v>
+        <v>179</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>303</v>
+        <v>180</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>301</v>
+        <v>183</v>
       </c>
       <c r="E69" s="9">
-        <v>5</v>
+        <v>34.979999999999997</v>
       </c>
       <c r="F69" s="9">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="G69" s="11" t="s">
-        <v>300</v>
-      </c>
-      <c r="H69" s="11" t="s">
-        <v>304</v>
+        <f>A69*E69</f>
+        <v>34.979999999999997</v>
+      </c>
+      <c r="G69" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="H69" s="10" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -18332,26 +18620,26 @@
         <v>1</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>179</v>
+        <v>206</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>180</v>
+        <v>207</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>183</v>
       </c>
       <c r="E70" s="9">
-        <v>34.979999999999997</v>
+        <v>10.99</v>
       </c>
       <c r="F70" s="9">
-        <f>A70*E70</f>
-        <v>34.979999999999997</v>
+        <f>E70*A70</f>
+        <v>10.99</v>
       </c>
       <c r="G70" s="10" t="s">
-        <v>182</v>
+        <v>208</v>
       </c>
       <c r="H70" s="10" t="s">
-        <v>181</v>
+        <v>209</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -18359,135 +18647,135 @@
         <v>1</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>183</v>
       </c>
       <c r="E71" s="9">
-        <v>10.99</v>
+        <v>61.9</v>
       </c>
       <c r="F71" s="9">
         <f>E71*A71</f>
-        <v>10.99</v>
+        <v>61.9</v>
       </c>
       <c r="G71" s="10" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="H71" s="10" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>200</v>
+        <v>293</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>201</v>
+        <v>36</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>183</v>
+        <v>74</v>
       </c>
       <c r="E72" s="9">
-        <v>61.9</v>
+        <v>1.6</v>
       </c>
       <c r="F72" s="9">
         <f>E72*A72</f>
-        <v>61.9</v>
+        <v>16</v>
       </c>
       <c r="G72" s="10" t="s">
-        <v>202</v>
+        <v>75</v>
       </c>
       <c r="H72" s="10" t="s">
-        <v>203</v>
+        <v>220</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
-        <v>10</v>
+        <v>138</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>293</v>
+        <v>3</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>36</v>
+        <v>155</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>74</v>
       </c>
       <c r="E73" s="9">
-        <v>1.6</v>
+        <f>7.5/100</f>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="F73" s="9">
-        <f>E73*A73</f>
-        <v>16</v>
+        <f>7.5*2</f>
+        <v>15</v>
       </c>
       <c r="G73" s="10" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="H73" s="10" t="s">
-        <v>220</v>
+        <v>81</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
-        <v>138</v>
+        <v>4</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>3</v>
+        <v>294</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>155</v>
+        <v>295</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>74</v>
       </c>
       <c r="E74" s="9">
-        <f>7.5/100</f>
-        <v>7.4999999999999997E-2</v>
+        <f>(0.85/5)*6</f>
+        <v>1.02</v>
       </c>
       <c r="F74" s="9">
-        <f>7.5*2</f>
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="G74" s="10" t="s">
-        <v>80</v>
+        <v>156</v>
       </c>
       <c r="H74" s="10" t="s">
-        <v>81</v>
+        <v>219</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" ht="27" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>295</v>
+        <v>217</v>
       </c>
       <c r="D75" s="4" t="s">
         <v>74</v>
       </c>
       <c r="E75" s="9">
-        <f>(0.85/5)*6</f>
-        <v>1.02</v>
+        <v>0.35</v>
       </c>
       <c r="F75" s="9">
-        <v>6</v>
+        <f>E75*A75</f>
+        <v>0.7</v>
       </c>
       <c r="G75" s="10" t="s">
-        <v>156</v>
+        <v>216</v>
       </c>
       <c r="H75" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="27" x14ac:dyDescent="0.25">
@@ -18495,80 +18783,80 @@
         <v>2</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>296</v>
+        <v>12</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>217</v>
+        <v>233</v>
       </c>
       <c r="D76" s="4" t="s">
         <v>74</v>
       </c>
       <c r="E76" s="9">
-        <v>0.35</v>
+        <v>1.5</v>
       </c>
       <c r="F76" s="9">
         <f>E76*A76</f>
-        <v>0.7</v>
+        <v>3</v>
       </c>
       <c r="G76" s="10" t="s">
-        <v>216</v>
+        <v>234</v>
       </c>
       <c r="H76" s="10" t="s">
-        <v>218</v>
+        <v>235</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="27" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>12</v>
+        <v>191</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>233</v>
+        <v>192</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>74</v>
+        <v>193</v>
       </c>
       <c r="E77" s="9">
-        <v>1.5</v>
+        <v>6.6</v>
       </c>
       <c r="F77" s="9">
         <f>E77*A77</f>
-        <v>3</v>
+        <v>6.6</v>
       </c>
       <c r="G77" s="10" t="s">
-        <v>234</v>
+        <v>195</v>
       </c>
       <c r="H77" s="10" t="s">
-        <v>235</v>
+        <v>194</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>191</v>
+        <v>334</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>192</v>
+        <v>335</v>
       </c>
       <c r="D78" s="4" t="s">
         <v>193</v>
       </c>
       <c r="E78" s="9">
-        <v>6.6</v>
+        <v>10.9</v>
       </c>
       <c r="F78" s="9">
         <f>E78*A78</f>
-        <v>6.6</v>
+        <v>21.8</v>
       </c>
       <c r="G78" s="10" t="s">
-        <v>195</v>
-      </c>
-      <c r="H78" s="10" t="s">
-        <v>194</v>
+        <v>336</v>
+      </c>
+      <c r="H78" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -18898,13 +19186,13 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
-        <v>121</v>
+        <v>6</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="D92" s="4" t="s">
         <v>106</v>
@@ -18914,74 +19202,74 @@
         <v>4.6666666666666669E-2</v>
       </c>
       <c r="F92" s="9">
-        <f>11*0.56</f>
-        <v>6.16</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="G92" s="10" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="H92" s="10"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
-        <v>26</v>
+        <v>121</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D93" s="4" t="s">
         <v>106</v>
       </c>
       <c r="E93" s="9">
-        <f>0.66/12</f>
-        <v>5.5E-2</v>
+        <f>0.56/12</f>
+        <v>4.6666666666666669E-2</v>
       </c>
       <c r="F93" s="9">
-        <f>3*0.66</f>
-        <v>1.98</v>
+        <f>11*0.56</f>
+        <v>6.16</v>
       </c>
       <c r="G93" s="10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H93" s="10"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D94" s="4" t="s">
         <v>106</v>
       </c>
       <c r="E94" s="9">
-        <f>0.67/12</f>
-        <v>5.5833333333333339E-2</v>
+        <f>0.66/12</f>
+        <v>5.5E-2</v>
       </c>
       <c r="F94" s="9">
-        <v>0.67</v>
+        <f>3*0.66</f>
+        <v>1.98</v>
       </c>
       <c r="G94" s="10" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H94" s="10"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D95" s="4" t="s">
         <v>106</v>
@@ -18994,344 +19282,389 @@
         <v>0.67</v>
       </c>
       <c r="G95" s="10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H95" s="10"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>298</v>
+        <v>4</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>299</v>
+        <v>145</v>
       </c>
       <c r="D96" s="4" t="s">
         <v>106</v>
       </c>
       <c r="E96" s="9">
-        <f>0.69/12</f>
-        <v>5.7499999999999996E-2</v>
+        <f>0.67/12</f>
+        <v>5.5833333333333339E-2</v>
       </c>
       <c r="F96" s="9">
-        <v>0.69</v>
+        <v>0.67</v>
       </c>
       <c r="G96" s="10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H96" s="10"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>25</v>
+        <v>298</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>148</v>
+        <v>299</v>
       </c>
       <c r="D97" s="4" t="s">
         <v>106</v>
       </c>
       <c r="E97" s="9">
-        <f>0.84/12</f>
-        <v>6.9999999999999993E-2</v>
+        <f>0.69/12</f>
+        <v>5.7499999999999996E-2</v>
       </c>
       <c r="F97" s="9">
-        <v>0.84</v>
+        <v>0.69</v>
       </c>
       <c r="G97" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H97" s="10"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>149</v>
+        <v>25</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D98" s="4" t="s">
         <v>106</v>
       </c>
       <c r="E98" s="9">
-        <f>0.56/12</f>
-        <v>4.6666666666666669E-2</v>
+        <f>0.84/12</f>
+        <v>6.9999999999999993E-2</v>
       </c>
       <c r="F98" s="9">
-        <v>0.56000000000000005</v>
+        <v>0.84</v>
       </c>
       <c r="G98" s="10" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H98" s="10"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>241</v>
+        <v>164</v>
       </c>
       <c r="D99" s="4" t="s">
         <v>106</v>
       </c>
       <c r="E99" s="9">
-        <f>0.15/25</f>
-        <v>6.0000000000000001E-3</v>
+        <f>0.44/4</f>
+        <v>0.11</v>
       </c>
       <c r="F99" s="9">
-        <v>0.15</v>
+        <f>E99*A99</f>
+        <v>0.44</v>
       </c>
       <c r="G99" s="10" t="s">
-        <v>236</v>
-      </c>
-      <c r="H99" s="10"/>
+        <v>341</v>
+      </c>
+      <c r="H99" s="10" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>8</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D100" s="4" t="s">
         <v>106</v>
       </c>
       <c r="E100" s="9">
-        <f>0.41/25</f>
-        <v>1.6399999999999998E-2</v>
+        <f>0.15/25</f>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="F100" s="9">
-        <v>0.41</v>
+        <v>0.15</v>
       </c>
       <c r="G100" s="10" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="H100" s="10"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>54</v>
+        <v>11</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D101" s="4" t="s">
         <v>106</v>
       </c>
       <c r="E101" s="9">
-        <f>0.66/25</f>
-        <v>2.64E-2</v>
+        <f>0.41/25</f>
+        <v>1.6399999999999998E-2</v>
       </c>
       <c r="F101" s="9">
-        <v>0.66</v>
+        <v>0.41</v>
       </c>
       <c r="G101" s="10" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="H101" s="10"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D102" s="4" t="s">
         <v>106</v>
       </c>
       <c r="E102" s="9">
-        <f>0.64/25</f>
-        <v>2.5600000000000001E-2</v>
+        <f>0.66/25</f>
+        <v>2.64E-2</v>
       </c>
       <c r="F102" s="9">
-        <v>0.64</v>
+        <v>0.66</v>
       </c>
       <c r="G102" s="10" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H102" s="10"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D103" s="4" t="s">
         <v>106</v>
       </c>
       <c r="E103" s="9">
-        <f>0.2/25</f>
-        <v>8.0000000000000002E-3</v>
+        <f>0.64/25</f>
+        <v>2.5600000000000001E-2</v>
       </c>
       <c r="F103" s="9">
-        <v>0.2</v>
+        <v>0.64</v>
       </c>
       <c r="G103" s="10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H103" s="10"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D104" s="4" t="s">
         <v>106</v>
       </c>
       <c r="E104" s="9">
-        <f>0.56/25</f>
-        <v>2.2400000000000003E-2</v>
+        <f>0.2/25</f>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="F104" s="9">
-        <v>0.56000000000000005</v>
+        <v>0.2</v>
       </c>
       <c r="G104" s="10" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="H104" s="10"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D105" s="4" t="s">
         <v>106</v>
       </c>
       <c r="E105" s="9">
+        <f>0.56/25</f>
+        <v>2.2400000000000003E-2</v>
+      </c>
+      <c r="F105" s="9">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="G105" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="H105" s="10"/>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A106" s="3">
+        <v>12</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="D106" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E106" s="9">
         <f>0.69/25</f>
         <v>2.76E-2</v>
       </c>
-      <c r="F105" s="9">
+      <c r="F106" s="9">
         <v>0.69</v>
       </c>
-      <c r="G105" s="10" t="s">
+      <c r="G106" s="10" t="s">
         <v>248</v>
       </c>
-      <c r="H105" s="10"/>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E107" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="F107" s="2">
-        <f>SUM(F2:F105)</f>
-        <v>1101.2520000000006</v>
-      </c>
+      <c r="H106" s="10"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B108" s="12" t="s">
+      <c r="E108" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="F108" s="2">
+        <f>SUM(F2:F106)</f>
+        <v>1117.2820000000006</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B109" s="12" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="109" spans="1:8" ht="27" x14ac:dyDescent="0.25">
-      <c r="A109">
-        <v>1</v>
-      </c>
-      <c r="B109" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="C109" s="8" t="s">
-        <v>307</v>
-      </c>
-      <c r="D109" s="7" t="s">
-        <v>309</v>
-      </c>
-      <c r="E109" s="1">
-        <v>60.12</v>
-      </c>
-      <c r="F109" s="1">
-        <f>E109*A109</f>
-        <v>60.12</v>
-      </c>
-      <c r="G109" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" ht="27" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>1</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>331</v>
+        <v>310</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>329</v>
+        <v>307</v>
       </c>
       <c r="D110" s="7" t="s">
-        <v>190</v>
+        <v>309</v>
       </c>
       <c r="E110" s="1">
-        <v>155</v>
+        <v>60.12</v>
       </c>
       <c r="F110" s="1">
         <f>E110*A110</f>
+        <v>60.12</v>
+      </c>
+      <c r="G110" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>1</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="C111" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="D111" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="E111" s="1">
         <v>155</v>
       </c>
-      <c r="G110" t="s">
+      <c r="F111" s="1">
+        <f>E111*A111</f>
+        <v>155</v>
+      </c>
+      <c r="G111" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B112" s="13" t="s">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B113" s="13" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="113" spans="2:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="B113" s="7" t="s">
+    <row r="114" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="B114" s="7" t="s">
         <v>312</v>
       </c>
-      <c r="C113" s="8" t="s">
+      <c r="C114" s="8" t="s">
         <v>332</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B116" s="13" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A117" s="17" t="s">
+        <v>339</v>
+      </c>
+      <c r="B117" s="8" t="s">
+        <v>340</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H105" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:H106" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H106">
+      <sortCondition ref="D1:D106"/>
+    </sortState>
+  </autoFilter>
   <customSheetViews>
     <customSheetView guid="{558925EA-5CF7-4433-B1B3-D7D45C0B5112}" showAutoFilter="1">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="D114" sqref="D114"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-      <autoFilter ref="A1:H1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
+      <autoFilter ref="A1:H106" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19341,41 +19674,41 @@
 
 <file path=xl/worksheets/wsSortMap1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheetSortMap xmlns="http://schemas.microsoft.com/office/excel/2006/main">
-  <rowSortMap ref="A2:IV105" count="103">
-    <row newVal="1" oldVal="45"/>
-    <row newVal="2" oldVal="61"/>
-    <row newVal="3" oldVal="42"/>
-    <row newVal="4" oldVal="41"/>
-    <row newVal="5" oldVal="79"/>
-    <row newVal="6" oldVal="80"/>
-    <row newVal="7" oldVal="82"/>
-    <row newVal="8" oldVal="46"/>
-    <row newVal="9" oldVal="49"/>
-    <row newVal="10" oldVal="44"/>
-    <row newVal="11" oldVal="77"/>
-    <row newVal="12" oldVal="89"/>
-    <row newVal="13" oldVal="98"/>
-    <row newVal="14" oldVal="92"/>
-    <row newVal="15" oldVal="43"/>
-    <row newVal="16" oldVal="84"/>
+  <rowSortMap ref="A2:IV107" count="106">
+    <row newVal="1" oldVal="61"/>
+    <row newVal="2" oldVal="42"/>
+    <row newVal="3" oldVal="41"/>
+    <row newVal="4" oldVal="81"/>
+    <row newVal="5" oldVal="82"/>
+    <row newVal="6" oldVal="84"/>
+    <row newVal="7" oldVal="46"/>
+    <row newVal="8" oldVal="49"/>
+    <row newVal="9" oldVal="91"/>
+    <row newVal="10" oldVal="100"/>
+    <row newVal="11" oldVal="94"/>
+    <row newVal="12" oldVal="43"/>
+    <row newVal="13" oldVal="44"/>
+    <row newVal="14" oldVal="45"/>
+    <row newVal="15" oldVal="86"/>
+    <row newVal="16" oldVal="79"/>
     <row newVal="17" oldVal="66"/>
     <row newVal="18" oldVal="71"/>
-    <row newVal="19" oldVal="87"/>
-    <row newVal="20" oldVal="100"/>
+    <row newVal="19" oldVal="89"/>
+    <row newVal="20" oldVal="102"/>
     <row newVal="21" oldVal="20"/>
     <row newVal="22" oldVal="27"/>
     <row newVal="23" oldVal="28"/>
     <row newVal="24" oldVal="75"/>
     <row newVal="25" oldVal="33"/>
     <row newVal="26" oldVal="47"/>
-    <row newVal="27" oldVal="104"/>
-    <row newVal="28" oldVal="99"/>
-    <row newVal="29" oldVal="85"/>
+    <row newVal="27" oldVal="106"/>
+    <row newVal="28" oldVal="101"/>
+    <row newVal="29" oldVal="87"/>
     <row newVal="30" oldVal="22"/>
     <row newVal="31" oldVal="76"/>
-    <row newVal="32" oldVal="93"/>
-    <row newVal="33" oldVal="88"/>
-    <row newVal="34" oldVal="94"/>
+    <row newVal="32" oldVal="95"/>
+    <row newVal="33" oldVal="90"/>
+    <row newVal="34" oldVal="96"/>
     <row newVal="35" oldVal="50"/>
     <row newVal="36" oldVal="1"/>
     <row newVal="37" oldVal="2"/>
@@ -19388,63 +19721,66 @@
     <row newVal="44" oldVal="13"/>
     <row newVal="45" oldVal="62"/>
     <row newVal="46" oldVal="32"/>
-    <row newVal="47" oldVal="64"/>
-    <row newVal="48" oldVal="52"/>
-    <row newVal="49" oldVal="67"/>
-    <row newVal="50" oldVal="36"/>
+    <row newVal="47" oldVal="52"/>
+    <row newVal="48" oldVal="67"/>
+    <row newVal="49" oldVal="36"/>
+    <row newVal="50" oldVal="64"/>
     <row newVal="51" oldVal="35"/>
     <row newVal="52" oldVal="70"/>
     <row newVal="53" oldVal="56"/>
-    <row newVal="54" oldVal="37"/>
-    <row newVal="55" oldVal="10"/>
-    <row newVal="56" oldVal="8"/>
-    <row newVal="57" oldVal="5"/>
-    <row newVal="58" oldVal="3"/>
-    <row newVal="59" oldVal="7"/>
-    <row newVal="60" oldVal="19"/>
-    <row newVal="61" oldVal="34"/>
-    <row newVal="62" oldVal="26"/>
-    <row newVal="63" oldVal="60"/>
-    <row newVal="64" oldVal="65"/>
-    <row newVal="65" oldVal="73"/>
-    <row newVal="66" oldVal="96"/>
-    <row newVal="67" oldVal="97"/>
-    <row newVal="68" oldVal="78"/>
-    <row newVal="69" oldVal="48"/>
-    <row newVal="70" oldVal="53"/>
-    <row newVal="71" oldVal="55"/>
-    <row newVal="72" oldVal="63"/>
-    <row newVal="73" oldVal="9"/>
-    <row newVal="75" oldVal="81"/>
-    <row newVal="76" oldVal="21"/>
-    <row newVal="77" oldVal="83"/>
-    <row newVal="78" oldVal="72"/>
-    <row newVal="79" oldVal="91"/>
-    <row newVal="80" oldVal="58"/>
-    <row newVal="81" oldVal="59"/>
-    <row newVal="82" oldVal="86"/>
-    <row newVal="83" oldVal="95"/>
-    <row newVal="84" oldVal="25"/>
-    <row newVal="85" oldVal="54"/>
-    <row newVal="86" oldVal="17"/>
-    <row newVal="87" oldVal="57"/>
-    <row newVal="88" oldVal="68"/>
-    <row newVal="89" oldVal="102"/>
-    <row newVal="90" oldVal="101"/>
-    <row newVal="91" oldVal="6"/>
-    <row newVal="92" oldVal="31"/>
-    <row newVal="93" oldVal="24"/>
-    <row newVal="94" oldVal="11"/>
-    <row newVal="95" oldVal="30"/>
-    <row newVal="96" oldVal="40"/>
-    <row newVal="97" oldVal="90"/>
-    <row newVal="98" oldVal="69"/>
-    <row newVal="99" oldVal="18"/>
-    <row newVal="100" oldVal="103"/>
-    <row newVal="101" oldVal="38"/>
-    <row newVal="102" oldVal="39"/>
-    <row newVal="103" oldVal="23"/>
-    <row newVal="104" oldVal="29"/>
+    <row newVal="54" oldVal="10"/>
+    <row newVal="55" oldVal="8"/>
+    <row newVal="56" oldVal="7"/>
+    <row newVal="57" oldVal="19"/>
+    <row newVal="58" oldVal="34"/>
+    <row newVal="59" oldVal="5"/>
+    <row newVal="60" oldVal="3"/>
+    <row newVal="61" oldVal="26"/>
+    <row newVal="62" oldVal="60"/>
+    <row newVal="63" oldVal="65"/>
+    <row newVal="64" oldVal="73"/>
+    <row newVal="65" oldVal="98"/>
+    <row newVal="66" oldVal="99"/>
+    <row newVal="67" oldVal="80"/>
+    <row newVal="68" oldVal="48"/>
+    <row newVal="69" oldVal="53"/>
+    <row newVal="70" oldVal="55"/>
+    <row newVal="71" oldVal="63"/>
+    <row newVal="72" oldVal="9"/>
+    <row newVal="73" oldVal="74"/>
+    <row newVal="74" oldVal="83"/>
+    <row newVal="75" oldVal="21"/>
+    <row newVal="76" oldVal="77"/>
+    <row newVal="77" oldVal="78"/>
+    <row newVal="78" oldVal="85"/>
+    <row newVal="79" oldVal="72"/>
+    <row newVal="80" oldVal="93"/>
+    <row newVal="81" oldVal="58"/>
+    <row newVal="82" oldVal="59"/>
+    <row newVal="83" oldVal="88"/>
+    <row newVal="84" oldVal="97"/>
+    <row newVal="85" oldVal="25"/>
+    <row newVal="86" oldVal="54"/>
+    <row newVal="87" oldVal="17"/>
+    <row newVal="88" oldVal="57"/>
+    <row newVal="89" oldVal="68"/>
+    <row newVal="90" oldVal="104"/>
+    <row newVal="91" oldVal="40"/>
+    <row newVal="92" oldVal="103"/>
+    <row newVal="93" oldVal="6"/>
+    <row newVal="94" oldVal="31"/>
+    <row newVal="95" oldVal="24"/>
+    <row newVal="96" oldVal="11"/>
+    <row newVal="97" oldVal="30"/>
+    <row newVal="98" oldVal="37"/>
+    <row newVal="99" oldVal="92"/>
+    <row newVal="100" oldVal="69"/>
+    <row newVal="101" oldVal="18"/>
+    <row newVal="102" oldVal="105"/>
+    <row newVal="103" oldVal="38"/>
+    <row newVal="104" oldVal="39"/>
+    <row newVal="105" oldVal="23"/>
+    <row newVal="106" oldVal="29"/>
   </rowSortMap>
 </worksheetSortMap>
 </file>
</xml_diff>